<commit_message>
created A assertion class and implement though calling it in test classes.
</commit_message>
<xml_diff>
--- a/data/datasheet.xlsx
+++ b/data/datasheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EateasyTest\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AutomationTest\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBFF568A-880F-4323-8B92-186C98FE4419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47793D7-217E-4F24-9F25-5B9FE695EED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{189B9495-B78D-4443-8CA9-6F83967203BE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>username</t>
   </si>
@@ -34,23 +34,55 @@
     <t>password</t>
   </si>
   <si>
-    <t>ritesh</t>
-  </si>
-  <si>
     <t>akash</t>
   </si>
   <si>
     <t>sathish</t>
+  </si>
+  <si>
+    <t>useremail</t>
+  </si>
+  <si>
+    <t>Testing@123</t>
+  </si>
+  <si>
+    <t>Testing@1234</t>
+  </si>
+  <si>
+    <t>dummytesting@gmail.com</t>
+  </si>
+  <si>
+    <t>dummytesting1@gmail.com</t>
+  </si>
+  <si>
+    <t>kumar</t>
+  </si>
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>bnmb</t>
+  </si>
+  <si>
+    <t>sdff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -73,13 +105,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -392,10 +427,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B6883-2D9C-4A72-AA56-71461BA0DFB9}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{78730866-0FF1-4182-B012-3A3EC606B588}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{5AFFEAA8-F2B7-406B-9C01-10D40D315421}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{B4DD7B27-8987-4F57-A955-E257195BAAF5}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{7714A216-E863-4099-98B3-46CEC2C3CD71}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C671DB-B9C9-4564-B85C-2335C5EF957F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,49 +509,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2C671DB-B9C9-4564-B85C-2335C5EF957F}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
parallel done with multiple browser's
</commit_message>
<xml_diff>
--- a/data/datasheet.xlsx
+++ b/data/datasheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AutomationTest\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium_Test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47793D7-217E-4F24-9F25-5B9FE695EED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D0F85A-EE4B-4831-B80E-7420B3AA096F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{189B9495-B78D-4443-8CA9-6F83967203BE}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>username</t>
   </si>
@@ -46,25 +46,37 @@
     <t>Testing@123</t>
   </si>
   <si>
+    <t>dummytesting@gmail.com</t>
+  </si>
+  <si>
+    <t>kumar</t>
+  </si>
+  <si>
+    <t>sam</t>
+  </si>
+  <si>
+    <t>dummytesting1@gmail.com</t>
+  </si>
+  <si>
     <t>Testing@1234</t>
   </si>
   <si>
-    <t>dummytesting@gmail.com</t>
-  </si>
-  <si>
-    <t>dummytesting1@gmail.com</t>
-  </si>
-  <si>
-    <t>kumar</t>
-  </si>
-  <si>
-    <t>sam</t>
-  </si>
-  <si>
-    <t>bnmb</t>
-  </si>
-  <si>
-    <t>sdff</t>
+    <t>mndbmfnb</t>
+  </si>
+  <si>
+    <t>dsfbsdnfb</t>
+  </si>
+  <si>
+    <t>fjsdfh</t>
+  </si>
+  <si>
+    <t>hkjhkjh</t>
+  </si>
+  <si>
+    <t>yweiruy</t>
+  </si>
+  <si>
+    <t>sdhfkjhsd</t>
   </si>
 </sst>
 </file>
@@ -427,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209B6883-2D9C-4A72-AA56-71461BA0DFB9}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +460,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -456,10 +468,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,14 +480,30 @@
       </c>
       <c r="B4" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{78730866-0FF1-4182-B012-3A3EC606B588}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{5AFFEAA8-F2B7-406B-9C01-10D40D315421}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{B4DD7B27-8987-4F57-A955-E257195BAAF5}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{7714A216-E863-4099-98B3-46CEC2C3CD71}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{30AF13B7-D62B-4266-9080-A01B56E6FC31}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{C0F08523-AF37-4A0B-B352-9FAD5B281394}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -486,7 +514,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,7 +537,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -517,10 +545,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>